<commit_message>
updated the task excel file
</commit_message>
<xml_diff>
--- a/proj todo.xlsx
+++ b/proj todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c43b1c1bd6959e9d/Desktop/studywork/SL/proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{37C97CF4-D1FC-4935-8CA8-56AA60DAD621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF0A1ED9-9260-43EE-A1A4-D6A0F3D5CF40}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{37C97CF4-D1FC-4935-8CA8-56AA60DAD621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF48B5AB-0662-4AE0-B64B-0F05DCA600D1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7BC7525E-6403-43EB-AEA6-D7781C41A931}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Hospital management system</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>made a sample run with the scheduled job</t>
+  </si>
+  <si>
+    <t>Created index.php and made it to fetch the data from database and send the data back to frontend in json format</t>
+  </si>
+  <si>
+    <t>updated the Results.js to receive the data from backend and populate it in a table.</t>
   </si>
 </sst>
 </file>
@@ -169,6 +175,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,10 +544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01F99E6-F4FC-4C10-99FD-1327C3077E0E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,6 +606,28 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>45581</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>45581</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>